<commit_message>
2021-3-31 p.m. slam learn
</commit_message>
<xml_diff>
--- a/Slam/2_slam_paper.xlsx
+++ b/Slam/2_slam_paper.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>title</t>
   </si>
@@ -36,6 +36,9 @@
     <t>comments</t>
   </si>
   <si>
+    <t>direction inspiration</t>
+  </si>
+  <si>
     <t>Past, Present, and Future of Simultaneous Localization And Mapping Towards the Robust-Perception Age</t>
   </si>
   <si>
@@ -43,6 +46,25 @@
   </si>
   <si>
     <t>IEEE Transactions on Robotics</t>
+  </si>
+  <si>
+    <t>无人系统视觉SLAM技术发展现状简析</t>
+  </si>
+  <si>
+    <t>李云天, 穆荣军, 单永志</t>
+  </si>
+  <si>
+    <t>控制与决策</t>
+  </si>
+  <si>
+    <t>1.前端：特征法和直接法；2.后端：非线性滤波优化；3.视觉/惯性SLAM技术研究现状；4.开源vSLAM框架对比分析；5. 挑战：动态适应性、泛化能力、高级感知能力、多传感器融合</t>
+  </si>
+  <si>
+    <t>不错的中文V-SLAM版 论文1</t>
+  </si>
+  <si>
+    <t>事件相机有望成为继RGB-D相机后的新型视觉传感器；深度学习在特征提取、回环检测等方面大放异彩；语义
+辅助vSLAM的研究成果稍逊一筹.目前语义vSLAM的相关研究尚不完善,但是最具潜力研究方向之一</t>
   </si>
 </sst>
 </file>
@@ -52,8 +74,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -79,6 +101,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +125,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -102,7 +139,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -110,37 +162,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,21 +183,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -193,6 +207,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -202,7 +217,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,7 +239,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,61 +260,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,115 +434,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,21 +460,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -463,6 +470,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,11 +516,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,10 +553,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -543,31 +565,37 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -576,104 +604,98 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -681,6 +703,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1031,24 +1056,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="63.4444444444444" style="1" customWidth="1"/>
+    <col min="1" max="1" width="62.3333333333333" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.5555555555556" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.5555555555556" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.3333333333333" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6666666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="73.8888888888889" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.2222222222222" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="20.6666666666667" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" ht="31.2" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1066,25 +1092,52 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" ht="109.2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>2016</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" ht="171.6" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="Past, Present, and Future of Simultaneous Localization And Mapping Towards the Robust-Perception Age" tooltip="Past, Present, and Future of Simultaneous Localization And Mapping Towards the Robust-Perception Age"/>
+    <hyperlink ref="A3" r:id="rId2" display="无人系统视觉SLAM技术发展现状简析"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
2021-4-1 p.m. slam learn
</commit_message>
<xml_diff>
--- a/Slam/2_slam_paper.xlsx
+++ b/Slam/2_slam_paper.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>title</t>
   </si>
@@ -65,6 +65,12 @@
   <si>
     <t>事件相机有望成为继RGB-D相机后的新型视觉传感器；深度学习在特征提取、回环检测等方面大放异彩；语义
 辅助vSLAM的研究成果稍逊一筹.目前语义vSLAM的相关研究尚不完善,但是最具潜力研究方向之一</t>
+  </si>
+  <si>
+    <t>A Survey of Simultaneous Localizationand Mapping SLAM.pdf</t>
+  </si>
+  <si>
+    <t>Baichuan Huang等</t>
   </si>
 </sst>
 </file>
@@ -73,9 +79,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -109,8 +115,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -124,6 +158,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -132,44 +167,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,9 +181,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,6 +228,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -209,37 +245,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,181 +260,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,15 +480,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -494,6 +491,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -530,21 +551,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -553,10 +559,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -565,133 +571,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1056,13 +1062,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelRow="3" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="62.3333333333333" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.5555555555556" style="1" customWidth="1"/>
@@ -1134,10 +1140,22 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2020</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="Past, Present, and Future of Simultaneous Localization And Mapping Towards the Robust-Perception Age" tooltip="Past, Present, and Future of Simultaneous Localization And Mapping Towards the Robust-Perception Age"/>
     <hyperlink ref="A3" r:id="rId2" display="无人系统视觉SLAM技术发展现状简析"/>
+    <hyperlink ref="A4" r:id="rId3" display="A Survey of Simultaneous Localizationand Mapping SLAM.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>